<commit_message>
fix naming consistency IsCloudK vs IsOnCloudK
</commit_message>
<xml_diff>
--- a/python/pdstools/resources/MetricLimits.xlsx
+++ b/python/pdstools/resources/MetricLimits.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pegasystems.sharepoint.com/sites/SP-PRD-1-1CustomerEngagementAlliance/Chapters/AI Chapter/projects/Client Intelligence/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vanej/Library/CloudStorage/OneDrive-PegasystemsInc/Documents/code/pega-datascientist-tools/python/pdstools/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="244" documentId="8_{A228393B-BD44-9544-A227-413E1768BFD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7525C9DE-8E85-6E46-9303-29C83E2B0E1C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{409A8F6D-8187-F04D-9108-60109607DA88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19680" yWindow="-23500" windowWidth="34480" windowHeight="19560" xr2:uid="{4A8314C0-E379-8446-B48C-F7C285D6E242}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20600" xr2:uid="{4A8314C0-E379-8446-B48C-F7C285D6E242}"/>
   </bookViews>
   <sheets>
     <sheet name="Thresholds" sheetId="1" r:id="rId1"/>
@@ -95,9 +95,6 @@
     <t>Environment</t>
   </si>
   <si>
-    <t>IsOnCloudK</t>
-  </si>
-  <si>
     <t>IsPegaCloud</t>
   </si>
   <si>
@@ -231,6 +228,9 @@
   </si>
   <si>
     <t>UsingImpactAnalyzer</t>
+  </si>
+  <si>
+    <t>IsCloudK</t>
   </si>
 </sst>
 </file>
@@ -1151,7 +1151,7 @@
   <dimension ref="A1:H59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1205,7 +1205,7 @@
         <v>0.8</v>
       </c>
       <c r="G2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>10</v>
@@ -1248,7 +1248,7 @@
         <v>0.8</v>
       </c>
       <c r="G4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H4" s="5" t="s">
         <v>15</v>
@@ -1276,7 +1276,7 @@
         <v>18</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>19</v>
+        <v>64</v>
       </c>
       <c r="D6" t="b">
         <v>1</v>
@@ -1288,21 +1288,21 @@
         <v>18</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C7" t="b">
         <v>1</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
         <v>22</v>
-      </c>
-      <c r="B8" t="s">
-        <v>23</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -1314,18 +1314,18 @@
         <v>100</v>
       </c>
       <c r="G8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" s="5" t="s">
         <v>24</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -1337,10 +1337,10 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -1349,15 +1349,15 @@
         <v>200</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -1366,16 +1366,16 @@
         <v>200</v>
       </c>
       <c r="G11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H11" s="5"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -1387,10 +1387,10 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -1402,19 +1402,19 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H14" s="5"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C15" s="1">
         <v>0.05</v>
@@ -1432,18 +1432,18 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C17">
         <v>52</v>
@@ -1460,26 +1460,26 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C20" s="1">
         <v>0.01</v>
@@ -1491,15 +1491,15 @@
         <v>1</v>
       </c>
       <c r="G20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C21">
         <v>50</v>
@@ -1514,15 +1514,15 @@
         <v>2000</v>
       </c>
       <c r="G21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" t="s">
         <v>39</v>
-      </c>
-      <c r="B22" t="s">
-        <v>40</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -1533,34 +1533,34 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C26" t="b">
         <v>1</v>
@@ -1568,10 +1568,10 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D27" t="b">
         <v>1</v>
@@ -1579,10 +1579,10 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C28" t="b">
         <v>1</v>
@@ -1590,10 +1590,10 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B29" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D29" t="b">
         <v>1</v>
@@ -1601,10 +1601,10 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" s="4" t="s">
         <v>47</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>48</v>
       </c>
       <c r="C30">
         <v>50</v>
@@ -1619,15 +1619,15 @@
         <v>10000</v>
       </c>
       <c r="G30" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C31">
         <v>50</v>
@@ -1644,10 +1644,10 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -1659,15 +1659,15 @@
         <v>25</v>
       </c>
       <c r="G32" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B33" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -1679,23 +1679,23 @@
         <v>5</v>
       </c>
       <c r="G33" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -1709,10 +1709,10 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B36" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -1724,15 +1724,15 @@
         <v>25</v>
       </c>
       <c r="G36" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B37" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C37">
         <v>2</v>
@@ -1747,15 +1747,15 @@
         <v>5000</v>
       </c>
       <c r="G37" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C38">
         <v>2</v>
@@ -1770,7 +1770,7 @@
         <v>2500</v>
       </c>
       <c r="G38" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
@@ -2120,6 +2120,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="089cec44-d2e6-4cdf-ac62-07269f32bc9f">
@@ -2130,15 +2139,6 @@
     <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2162,6 +2162,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C20C73FF-AAF1-4BDD-9C40-B4772DF82186}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7BCD6B0-A36C-4B0E-9370-E7046D7BE05E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
@@ -2177,12 +2185,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C20C73FF-AAF1-4BDD-9C40-B4772DF82186}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
complemented metrics and limits
</commit_message>
<xml_diff>
--- a/python/pdstools/resources/MetricLimits.xlsx
+++ b/python/pdstools/resources/MetricLimits.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vanej/Library/CloudStorage/OneDrive-PegasystemsInc/Documents/code/pega-datascientist-tools/python/pdstools/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{409A8F6D-8187-F04D-9108-60109607DA88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB7B24D3-2DEA-A040-979B-AC7ABADB7811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20600" xr2:uid="{4A8314C0-E379-8446-B48C-F7C285D6E242}"/>
+    <workbookView xWindow="-19200" yWindow="-20480" windowWidth="34560" windowHeight="20600" xr2:uid="{4A8314C0-E379-8446-B48C-F7C285D6E242}"/>
   </bookViews>
   <sheets>
     <sheet name="Thresholds" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="70">
   <si>
     <t>Category</t>
   </si>
@@ -110,9 +110,6 @@
     <t>Per configuration?</t>
   </si>
   <si>
-    <t>Use either Best Practice Min or Max (or both) to give the GOOD value (which becomes green)</t>
-  </si>
-  <si>
     <t>DailyPositiveCount</t>
   </si>
   <si>
@@ -231,13 +228,31 @@
   </si>
   <si>
     <t>IsCloudK</t>
+  </si>
+  <si>
+    <t>InboundChannelCount</t>
+  </si>
+  <si>
+    <t>OutboundChannelCount</t>
+  </si>
+  <si>
+    <t>Use Minimum or Best Practice Min to indicate whether not satisfying is critical (RED) or not best practice (AMBER)</t>
+  </si>
+  <si>
+    <t>ClickThroughTrend</t>
+  </si>
+  <si>
+    <t>Some variance can occur so 0.96 can occur without alarm bells. Best practice is seeing growth</t>
+  </si>
+  <si>
+    <t>HasMLAIData</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -398,6 +413,12 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="6"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -696,7 +717,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -739,8 +760,9 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -752,9 +774,12 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -794,11 +819,27 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Percent" xfId="42" builtinId="5"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -812,15 +853,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C8831824-308D-534A-8FAC-51D6E4FA2EF5}" name="Table1" displayName="Table1" ref="A1:G38" totalsRowShown="0">
-  <autoFilter ref="A1:G38" xr:uid="{C8831824-308D-534A-8FAC-51D6E4FA2EF5}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G38">
-    <sortCondition ref="A2:A38"/>
-    <sortCondition ref="B2:B38"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C8831824-308D-534A-8FAC-51D6E4FA2EF5}" name="Table1" displayName="Table1" ref="A1:G42" totalsRowShown="0">
+  <autoFilter ref="A1:G42" xr:uid="{C8831824-308D-534A-8FAC-51D6E4FA2EF5}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G40">
+    <sortCondition ref="A2:A40"/>
+    <sortCondition ref="B2:B40"/>
   </sortState>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{F2760838-3016-C644-94CF-3772759AD80A}" name="Category"/>
-    <tableColumn id="3" xr3:uid="{571C1962-801F-3A43-9A27-919AD06806D5}" name="MetricID"/>
+    <tableColumn id="3" xr3:uid="{571C1962-801F-3A43-9A27-919AD06806D5}" name="MetricID" dataDxfId="0"/>
     <tableColumn id="4" xr3:uid="{8F777A7A-3E1C-B446-95D7-5C9D64D4E0F2}" name="Minimum"/>
     <tableColumn id="5" xr3:uid="{25EA7F58-34E2-1A47-836E-F1878A686E77}" name="Best Practice Min"/>
     <tableColumn id="6" xr3:uid="{C1AAFE35-8831-C54E-993C-4A4C2CB23FFE}" name="Best Practice Max"/>
@@ -1148,10 +1189,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE4ECA8F-C00F-5D41-BE9E-69A05050A68D}">
-  <dimension ref="A1:H59"/>
+  <dimension ref="A1:H61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1205,7 +1246,7 @@
         <v>0.8</v>
       </c>
       <c r="G2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>10</v>
@@ -1248,7 +1289,7 @@
         <v>0.8</v>
       </c>
       <c r="G4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H4" s="5" t="s">
         <v>15</v>
@@ -1276,7 +1317,7 @@
         <v>18</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D6" t="b">
         <v>1</v>
@@ -1299,39 +1340,36 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-      <c r="D8">
-        <v>5</v>
-      </c>
-      <c r="E8">
-        <v>100</v>
-      </c>
-      <c r="G8" t="s">
-        <v>23</v>
+        <v>18</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" t="b">
+        <v>1</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>24</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>25</v>
+      <c r="B9" s="7" t="s">
+        <v>22</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D9">
-        <v>200</v>
+        <v>5</v>
+      </c>
+      <c r="E9">
+        <v>100</v>
+      </c>
+      <c r="G9" t="s">
+        <v>23</v>
       </c>
       <c r="H9" s="5"/>
     </row>
@@ -1340,7 +1378,7 @@
         <v>21</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -1349,24 +1387,21 @@
         <v>200</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>21</v>
       </c>
-      <c r="B11" t="s">
-        <v>60</v>
+      <c r="B11" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11">
         <v>200</v>
-      </c>
-      <c r="G11" t="s">
-        <v>61</v>
       </c>
       <c r="H11" s="5"/>
     </row>
@@ -1374,14 +1409,17 @@
       <c r="A12" t="s">
         <v>21</v>
       </c>
-      <c r="B12" t="s">
-        <v>62</v>
+      <c r="B12" s="7" t="s">
+        <v>59</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
       <c r="D12">
         <v>200</v>
+      </c>
+      <c r="G12" t="s">
+        <v>60</v>
       </c>
       <c r="H12" s="5"/>
     </row>
@@ -1389,14 +1427,14 @@
       <c r="A13" t="s">
         <v>21</v>
       </c>
-      <c r="B13" t="s">
-        <v>28</v>
+      <c r="B13" s="7" t="s">
+        <v>61</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="H13" s="5"/>
     </row>
@@ -1404,8 +1442,14 @@
       <c r="A14" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>29</v>
+      <c r="B14" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
       </c>
       <c r="H14" s="5"/>
     </row>
@@ -1414,19 +1458,7 @@
         <v>21</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" s="1">
-        <v>0.05</v>
-      </c>
-      <c r="D15" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="E15" s="1">
-        <v>1</v>
-      </c>
-      <c r="G15" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="H15" s="5"/>
     </row>
@@ -1435,27 +1467,27 @@
         <v>21</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="E16" s="1">
+        <v>1</v>
+      </c>
+      <c r="G16" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>21</v>
       </c>
-      <c r="B17" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17">
-        <v>52</v>
-      </c>
-      <c r="D17">
-        <v>55</v>
-      </c>
-      <c r="E17">
-        <v>80</v>
-      </c>
-      <c r="F17">
-        <v>90</v>
+      <c r="B17" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -1463,7 +1495,19 @@
         <v>21</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
+      </c>
+      <c r="C18">
+        <v>52</v>
+      </c>
+      <c r="D18">
+        <v>55</v>
+      </c>
+      <c r="E18">
+        <v>80</v>
+      </c>
+      <c r="F18">
+        <v>90</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -1471,118 +1515,127 @@
         <v>21</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>21</v>
       </c>
-      <c r="B20" t="s">
-        <v>35</v>
-      </c>
-      <c r="C20" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="D20" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="E20" s="1">
-        <v>1</v>
-      </c>
-      <c r="G20" t="s">
-        <v>36</v>
+      <c r="B20" s="4" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>21</v>
       </c>
-      <c r="B21" t="s">
-        <v>57</v>
-      </c>
-      <c r="C21">
-        <v>50</v>
-      </c>
-      <c r="D21">
-        <v>200</v>
-      </c>
-      <c r="E21">
-        <v>700</v>
-      </c>
-      <c r="F21">
-        <v>2000</v>
+      <c r="B21" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="E21" s="1">
+        <v>1</v>
       </c>
       <c r="G21" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>38</v>
-      </c>
-      <c r="B22" t="s">
-        <v>39</v>
+        <v>21</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>56</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="D22">
-        <v>2</v>
+        <v>200</v>
+      </c>
+      <c r="E22">
+        <v>700</v>
+      </c>
+      <c r="F22">
+        <v>2000</v>
+      </c>
+      <c r="G22" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>40</v>
+        <v>67</v>
+      </c>
+      <c r="C23">
+        <v>0.95</v>
+      </c>
+      <c r="D23">
+        <v>1.05</v>
+      </c>
+      <c r="G23" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B24" s="4" t="s">
-        <v>41</v>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C26" t="b">
-        <v>1</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>38</v>
-      </c>
-      <c r="B27" t="s">
-        <v>44</v>
-      </c>
-      <c r="D27" t="b">
-        <v>1</v>
+        <v>37</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E27" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="F27" s="9">
+        <v>0.9</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C28" t="b">
         <v>1</v>
@@ -1590,10 +1643,10 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>38</v>
-      </c>
-      <c r="B29" t="s">
-        <v>63</v>
+        <v>37</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="D29" t="b">
         <v>1</v>
@@ -1601,186 +1654,233 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C30">
-        <v>50</v>
-      </c>
-      <c r="D30">
-        <v>100</v>
-      </c>
-      <c r="E30">
-        <v>2500</v>
-      </c>
-      <c r="F30">
-        <v>10000</v>
-      </c>
-      <c r="G30" t="s">
-        <v>48</v>
+        <v>44</v>
+      </c>
+      <c r="C30" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>46</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C31">
-        <v>50</v>
-      </c>
-      <c r="D31">
-        <v>100</v>
-      </c>
-      <c r="E31">
-        <v>2500</v>
-      </c>
-      <c r="F31">
-        <v>10000</v>
+        <v>37</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D31" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>45</v>
+      </c>
+      <c r="B32" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32">
         <v>50</v>
       </c>
-      <c r="C32">
-        <v>1</v>
-      </c>
       <c r="D32">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="E32">
-        <v>25</v>
+        <v>2500</v>
+      </c>
+      <c r="F32">
+        <v>10000</v>
       </c>
       <c r="G32" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>46</v>
-      </c>
-      <c r="B33" t="s">
-        <v>51</v>
+        <v>45</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="C33">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="D33">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="E33">
-        <v>5</v>
-      </c>
-      <c r="G33" t="s">
-        <v>48</v>
+        <v>2500</v>
+      </c>
+      <c r="F33">
+        <v>10000</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34">
+        <v>5</v>
+      </c>
+      <c r="E34">
+        <v>25</v>
+      </c>
+      <c r="G34" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>46</v>
-      </c>
-      <c r="B35" t="s">
-        <v>53</v>
+        <v>45</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>50</v>
       </c>
       <c r="C35">
         <v>1</v>
       </c>
       <c r="D35">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="E35">
-        <v>250</v>
+        <v>5</v>
+      </c>
+      <c r="G35" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>46</v>
-      </c>
-      <c r="B36" t="s">
-        <v>54</v>
-      </c>
-      <c r="C36">
-        <v>1</v>
-      </c>
-      <c r="D36">
-        <v>5</v>
-      </c>
-      <c r="E36">
-        <v>25</v>
-      </c>
-      <c r="G36" t="s">
-        <v>48</v>
+        <v>45</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>46</v>
-      </c>
-      <c r="B37" t="s">
-        <v>55</v>
+        <v>45</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>52</v>
       </c>
       <c r="C37">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D37">
-        <v>2500</v>
+        <v>100</v>
       </c>
       <c r="E37">
-        <v>5000</v>
-      </c>
-      <c r="F37">
-        <v>5000</v>
-      </c>
-      <c r="G37" t="s">
-        <v>48</v>
+        <v>250</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>46</v>
-      </c>
-      <c r="B38" t="s">
-        <v>56</v>
+        <v>45</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38">
+        <v>5</v>
+      </c>
+      <c r="E38">
+        <v>25</v>
+      </c>
+      <c r="G38" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>45</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C39">
         <v>2</v>
       </c>
-      <c r="D38">
+      <c r="D39">
+        <v>2500</v>
+      </c>
+      <c r="E39">
+        <v>5000</v>
+      </c>
+      <c r="F39">
+        <v>5000</v>
+      </c>
+      <c r="G39" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>45</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C40">
+        <v>2</v>
+      </c>
+      <c r="D40">
         <v>1000</v>
       </c>
-      <c r="E38">
+      <c r="E40">
         <v>2500</v>
       </c>
-      <c r="F38">
+      <c r="F40">
         <v>2500</v>
       </c>
-      <c r="G38" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40" s="2"/>
+      <c r="G40" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" s="2"/>
+      <c r="A41" t="s">
+        <v>45</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <v>50</v>
+      </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A42" s="2"/>
+      <c r="A42" t="s">
+        <v>45</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <v>50</v>
+      </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="2"/>
@@ -1807,13 +1907,13 @@
       <c r="A50" s="2"/>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A51" s="3"/>
+      <c r="A51" s="2"/>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" s="2"/>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A53" s="2"/>
+      <c r="A53" s="3"/>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" s="2"/>
@@ -1832,6 +1932,12 @@
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" s="2"/>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60" s="2"/>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A61" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2120,15 +2226,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="089cec44-d2e6-4cdf-ac62-07269f32bc9f">
@@ -2139,6 +2236,15 @@
     <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2162,14 +2268,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C20C73FF-AAF1-4BDD-9C40-B4772DF82186}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7BCD6B0-A36C-4B0E-9370-E7046D7BE05E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
@@ -2185,4 +2283,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C20C73FF-AAF1-4BDD-9C40-B4772DF82186}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update metrics and limits, add github workflow for writing csv (#502)
</commit_message>
<xml_diff>
--- a/python/pdstools/resources/MetricLimits.xlsx
+++ b/python/pdstools/resources/MetricLimits.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pegasystems.sharepoint.com/sites/SP-PRD-1-1CustomerEngagementAlliance/Chapters/AI Chapter/projects/Client Intelligence/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vanej/Library/CloudStorage/OneDrive-PegasystemsInc/Documents/code/pega-datascientist-tools/python/pdstools/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="244" documentId="8_{A228393B-BD44-9544-A227-413E1768BFD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7525C9DE-8E85-6E46-9303-29C83E2B0E1C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BA63E0A-7364-3E43-AE34-AB90AB29966D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19680" yWindow="-23500" windowWidth="34480" windowHeight="19560" xr2:uid="{4A8314C0-E379-8446-B48C-F7C285D6E242}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20600" xr2:uid="{4A8314C0-E379-8446-B48C-F7C285D6E242}"/>
   </bookViews>
   <sheets>
     <sheet name="Thresholds" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="71">
   <si>
     <t>Category</t>
   </si>
@@ -74,9 +74,6 @@
     <t>InboundOptionality</t>
   </si>
   <si>
-    <t>Green colored metrics currently available, black not (yet)</t>
-  </si>
-  <si>
     <t>Good values (green) are between Best Practice Min and Max (INCLUSIVE the min/max values)</t>
   </si>
   <si>
@@ -95,9 +92,6 @@
     <t>Environment</t>
   </si>
   <si>
-    <t>IsOnCloudK</t>
-  </si>
-  <si>
     <t>IsPegaCloud</t>
   </si>
   <si>
@@ -113,9 +107,6 @@
     <t>Per configuration?</t>
   </si>
   <si>
-    <t>Use either Best Practice Min or Max (or both) to give the GOOD value (which becomes green)</t>
-  </si>
-  <si>
     <t>DailyPositiveCount</t>
   </si>
   <si>
@@ -152,9 +143,6 @@
     <t>Percentage actions used across channels</t>
   </si>
   <si>
-    <t>We don’t have this per model category or overall, only by configuration</t>
-  </si>
-  <si>
     <t>NBA Configuration</t>
   </si>
   <si>
@@ -231,13 +219,43 @@
   </si>
   <si>
     <t>UsingImpactAnalyzer</t>
+  </si>
+  <si>
+    <t>IsCloudK</t>
+  </si>
+  <si>
+    <t>InboundChannelCount</t>
+  </si>
+  <si>
+    <t>OutboundChannelCount</t>
+  </si>
+  <si>
+    <t>Use Minimum or Best Practice Min to indicate whether not satisfying is critical (RED) or not best practice (AMBER)</t>
+  </si>
+  <si>
+    <t>ClickThroughTrend</t>
+  </si>
+  <si>
+    <t>Some variance can occur so 0.96 can occur without alarm bells. Best practice is seeing growth</t>
+  </si>
+  <si>
+    <t>HasMLAIData</t>
+  </si>
+  <si>
+    <t>Green colored metrics currently available black not (yet)</t>
+  </si>
+  <si>
+    <t>We don’t have this per model category or overall - only by configuration</t>
+  </si>
+  <si>
+    <t>IsOnPDC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -398,6 +416,12 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="6"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -696,7 +720,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -739,8 +763,9 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -752,9 +777,10 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -794,11 +820,27 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Percent" xfId="42" builtinId="5"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -812,15 +854,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C8831824-308D-534A-8FAC-51D6E4FA2EF5}" name="Table1" displayName="Table1" ref="A1:G38" totalsRowShown="0">
-  <autoFilter ref="A1:G38" xr:uid="{C8831824-308D-534A-8FAC-51D6E4FA2EF5}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G38">
-    <sortCondition ref="A2:A38"/>
-    <sortCondition ref="B2:B38"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C8831824-308D-534A-8FAC-51D6E4FA2EF5}" name="Thresholds" displayName="Thresholds" ref="A1:G43" totalsRowShown="0">
+  <autoFilter ref="A1:G43" xr:uid="{C8831824-308D-534A-8FAC-51D6E4FA2EF5}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G41">
+    <sortCondition ref="A2:A41"/>
+    <sortCondition ref="B2:B41"/>
   </sortState>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{F2760838-3016-C644-94CF-3772759AD80A}" name="Category"/>
-    <tableColumn id="3" xr3:uid="{571C1962-801F-3A43-9A27-919AD06806D5}" name="MetricID"/>
+    <tableColumn id="3" xr3:uid="{571C1962-801F-3A43-9A27-919AD06806D5}" name="MetricID" dataDxfId="0"/>
     <tableColumn id="4" xr3:uid="{8F777A7A-3E1C-B446-95D7-5C9D64D4E0F2}" name="Minimum"/>
     <tableColumn id="5" xr3:uid="{25EA7F58-34E2-1A47-836E-F1878A686E77}" name="Best Practice Min"/>
     <tableColumn id="6" xr3:uid="{C1AAFE35-8831-C54E-993C-4A4C2CB23FFE}" name="Best Practice Max"/>
@@ -1148,10 +1190,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE4ECA8F-C00F-5D41-BE9E-69A05050A68D}">
-  <dimension ref="A1:H59"/>
+  <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1205,7 +1247,7 @@
         <v>0.8</v>
       </c>
       <c r="G2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>10</v>
@@ -1225,10 +1267,10 @@
         <v>7</v>
       </c>
       <c r="G3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -1236,7 +1278,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -1248,10 +1290,10 @@
         <v>0.8</v>
       </c>
       <c r="G4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -1259,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -1268,15 +1310,15 @@
         <v>7</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="D6" t="b">
         <v>1</v>
@@ -1285,79 +1327,73 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>20</v>
       </c>
       <c r="C7" t="b">
         <v>1</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-      <c r="D8">
-        <v>5</v>
-      </c>
-      <c r="E8">
-        <v>100</v>
-      </c>
-      <c r="G8" t="s">
-        <v>24</v>
+        <v>17</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" t="b">
+        <v>1</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>25</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9">
+        <v>70</v>
+      </c>
+      <c r="C9" t="b">
         <v>1</v>
-      </c>
-      <c r="D9">
-        <v>200</v>
       </c>
       <c r="H9" s="5"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>5</v>
+      </c>
+      <c r="E10">
+        <v>100</v>
+      </c>
+      <c r="G10" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10">
-        <v>200</v>
-      </c>
       <c r="H10" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" t="s">
-        <v>61</v>
+        <v>20</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -1365,17 +1401,14 @@
       <c r="D11">
         <v>200</v>
       </c>
-      <c r="G11" t="s">
-        <v>62</v>
-      </c>
       <c r="H11" s="5"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" t="s">
-        <v>63</v>
+        <v>20</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -1387,403 +1420,479 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>200</v>
+      </c>
+      <c r="G13" t="s">
+        <v>58</v>
       </c>
       <c r="H13" s="5"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>30</v>
+        <v>20</v>
+      </c>
+      <c r="B14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>200</v>
       </c>
       <c r="H14" s="5"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" s="1">
-        <v>0.05</v>
-      </c>
-      <c r="D15" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="E15" s="1">
+        <v>20</v>
+      </c>
+      <c r="B15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
         <v>1</v>
-      </c>
-      <c r="G15" t="s">
-        <v>9</v>
       </c>
       <c r="H15" s="5"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17">
-        <v>52</v>
-      </c>
-      <c r="D17">
-        <v>55</v>
-      </c>
-      <c r="E17">
-        <v>80</v>
-      </c>
-      <c r="F17">
-        <v>90</v>
+        <v>20</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="E17" s="1">
+        <v>1</v>
+      </c>
+      <c r="G17" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
+      </c>
+      <c r="C19">
+        <v>52</v>
+      </c>
+      <c r="D19">
+        <v>55</v>
+      </c>
+      <c r="E19">
+        <v>80</v>
+      </c>
+      <c r="F19">
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" t="s">
-        <v>36</v>
-      </c>
-      <c r="C20" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="D20" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="E20" s="1">
-        <v>1</v>
-      </c>
-      <c r="G20" t="s">
-        <v>37</v>
+        <v>20</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" t="s">
-        <v>58</v>
-      </c>
-      <c r="C21">
-        <v>50</v>
-      </c>
-      <c r="D21">
-        <v>200</v>
-      </c>
-      <c r="E21">
-        <v>700</v>
-      </c>
-      <c r="F21">
-        <v>2000</v>
-      </c>
-      <c r="G21" t="s">
-        <v>38</v>
+        <v>20</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22">
+        <v>33</v>
+      </c>
+      <c r="C22" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="E22" s="1">
         <v>1</v>
       </c>
-      <c r="D22">
-        <v>2</v>
+      <c r="G22" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>39</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>41</v>
+        <v>20</v>
+      </c>
+      <c r="B23" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23">
+        <v>50</v>
+      </c>
+      <c r="D23">
+        <v>200</v>
+      </c>
+      <c r="E23">
+        <v>700</v>
+      </c>
+      <c r="F23">
+        <v>2000</v>
+      </c>
+      <c r="G23" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>42</v>
+        <v>65</v>
+      </c>
+      <c r="C24">
+        <v>0.95</v>
+      </c>
+      <c r="D24">
+        <v>1.05</v>
+      </c>
+      <c r="G24" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>39</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>43</v>
+        <v>35</v>
+      </c>
+      <c r="B25" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C26" t="b">
-        <v>1</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>39</v>
-      </c>
-      <c r="B27" t="s">
-        <v>45</v>
-      </c>
-      <c r="D27" t="b">
-        <v>1</v>
+        <v>35</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B28" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C28" t="b">
-        <v>1</v>
+      <c r="E28" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="F28" s="8">
+        <v>0.9</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>39</v>
-      </c>
-      <c r="B29" t="s">
-        <v>64</v>
-      </c>
-      <c r="D29" t="b">
+        <v>35</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C30">
-        <v>50</v>
-      </c>
-      <c r="D30">
-        <v>100</v>
-      </c>
-      <c r="E30">
-        <v>2500</v>
-      </c>
-      <c r="F30">
-        <v>10000</v>
-      </c>
-      <c r="G30" t="s">
-        <v>49</v>
+        <v>41</v>
+      </c>
+      <c r="D30" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C31">
-        <v>50</v>
-      </c>
-      <c r="D31">
-        <v>100</v>
-      </c>
-      <c r="E31">
-        <v>2500</v>
-      </c>
-      <c r="F31">
-        <v>10000</v>
+        <v>42</v>
+      </c>
+      <c r="C31" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="B32" t="s">
-        <v>51</v>
-      </c>
-      <c r="C32">
+        <v>60</v>
+      </c>
+      <c r="D32" t="b">
         <v>1</v>
-      </c>
-      <c r="D32">
-        <v>5</v>
-      </c>
-      <c r="E32">
-        <v>25</v>
-      </c>
-      <c r="G32" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>47</v>
-      </c>
-      <c r="B33" t="s">
-        <v>52</v>
+        <v>43</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>44</v>
       </c>
       <c r="C33">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="D33">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="E33">
-        <v>5</v>
+        <v>2500</v>
+      </c>
+      <c r="F33">
+        <v>10000</v>
       </c>
       <c r="G33" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>53</v>
+        <v>46</v>
+      </c>
+      <c r="C34">
+        <v>50</v>
+      </c>
+      <c r="D34">
+        <v>100</v>
+      </c>
+      <c r="E34">
+        <v>2500</v>
+      </c>
+      <c r="F34">
+        <v>10000</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
+        <v>43</v>
+      </c>
+      <c r="B35" s="4" t="s">
         <v>47</v>
-      </c>
-      <c r="B35" t="s">
-        <v>54</v>
       </c>
       <c r="C35">
         <v>1</v>
       </c>
       <c r="D35">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="E35">
-        <v>250</v>
+        <v>25</v>
+      </c>
+      <c r="G35" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B36" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C36">
         <v>1</v>
       </c>
       <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36">
         <v>5</v>
       </c>
-      <c r="E36">
-        <v>25</v>
-      </c>
       <c r="G36" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>47</v>
-      </c>
-      <c r="B37" t="s">
-        <v>56</v>
-      </c>
-      <c r="C37">
-        <v>2</v>
-      </c>
-      <c r="D37">
-        <v>2500</v>
-      </c>
-      <c r="E37">
-        <v>5000</v>
-      </c>
-      <c r="F37">
-        <v>5000</v>
-      </c>
-      <c r="G37" t="s">
+        <v>43</v>
+      </c>
+      <c r="B37" s="7" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B38" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38">
+        <v>100</v>
+      </c>
+      <c r="E38">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>43</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39">
+        <v>5</v>
+      </c>
+      <c r="E39">
+        <v>25</v>
+      </c>
+      <c r="G39" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>43</v>
+      </c>
+      <c r="B40" t="s">
+        <v>52</v>
+      </c>
+      <c r="C40">
         <v>2</v>
       </c>
-      <c r="D38">
+      <c r="D40">
+        <v>2500</v>
+      </c>
+      <c r="E40">
+        <v>5000</v>
+      </c>
+      <c r="F40">
+        <v>5000</v>
+      </c>
+      <c r="G40" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>43</v>
+      </c>
+      <c r="B41" t="s">
+        <v>53</v>
+      </c>
+      <c r="C41">
+        <v>2</v>
+      </c>
+      <c r="D41">
         <v>1000</v>
       </c>
-      <c r="E38">
+      <c r="E41">
         <v>2500</v>
       </c>
-      <c r="F38">
+      <c r="F41">
         <v>2500</v>
       </c>
-      <c r="G38" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40" s="2"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" s="2"/>
+      <c r="G41" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A42" s="2"/>
+      <c r="A42" t="s">
+        <v>43</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <v>50</v>
+      </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A43" s="2"/>
+      <c r="A43" t="s">
+        <v>43</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43">
+        <v>50</v>
+      </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="2"/>
@@ -1807,7 +1916,7 @@
       <c r="A50" s="2"/>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A51" s="3"/>
+      <c r="A51" s="2"/>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" s="2"/>
@@ -1816,7 +1925,7 @@
       <c r="A53" s="2"/>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A54" s="2"/>
+      <c r="A54" s="3"/>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" s="2"/>
@@ -1832,6 +1941,15 @@
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" s="2"/>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60" s="2"/>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A61" s="2"/>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A62" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1842,6 +1960,28 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="089cec44-d2e6-4cdf-ac62-07269f32bc9f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="1d9227fc-758c-4c6d-9eef-c3984f6cd4f8" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004F47B8AB733B764FA385BB20C5590851" ma:contentTypeVersion="21" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="649c562f76f5c1e39005e85db0d2653a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="089cec44-d2e6-4cdf-ac62-07269f32bc9f" xmlns:ns3="1d9227fc-758c-4c6d-9eef-c3984f6cd4f8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7b1126210d46bbbe83ce1ab28b32db24" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2119,44 +2259,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="089cec44-d2e6-4cdf-ac62-07269f32bc9f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="1d9227fc-758c-4c6d-9eef-c3984f6cd4f8" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{269293F1-9DCF-44D2-8263-6EB6BC10E045}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C20C73FF-AAF1-4BDD-9C40-B4772DF82186}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="089cec44-d2e6-4cdf-ac62-07269f32bc9f"/>
-    <ds:schemaRef ds:uri="1d9227fc-758c-4c6d-9eef-c3984f6cd4f8"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2180,9 +2286,21 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C20C73FF-AAF1-4BDD-9C40-B4772DF82186}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{269293F1-9DCF-44D2-8263-6EB6BC10E045}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="089cec44-d2e6-4cdf-ac62-07269f32bc9f"/>
+    <ds:schemaRef ds:uri="1d9227fc-758c-4c6d-9eef-c3984f6cd4f8"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update limits for model maturity
</commit_message>
<xml_diff>
--- a/python/pdstools/resources/MetricLimits.xlsx
+++ b/python/pdstools/resources/MetricLimits.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vanej/Library/CloudStorage/OneDrive-PegasystemsInc/Documents/code/pega-datascientist-tools/python/pdstools/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCBFA13B-D165-FB4C-8ECC-E5B9DF4D3E36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECCA9AFF-C18D-484A-B39B-A404E4AC31FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20600" xr2:uid="{4A8314C0-E379-8446-B48C-F7C285D6E242}"/>
   </bookViews>
@@ -1193,7 +1193,7 @@
   <dimension ref="A1:H62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="117" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1482,14 +1482,12 @@
         <v>28</v>
       </c>
       <c r="C17" s="1">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="D17" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="E17" s="1">
-        <v>1</v>
-      </c>
+        <v>0.8</v>
+      </c>
+      <c r="E17" s="1"/>
       <c r="G17" t="s">
         <v>9</v>
       </c>
@@ -1962,6 +1960,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="089cec44-d2e6-4cdf-ac62-07269f32bc9f">
@@ -1972,15 +1979,6 @@
     <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2262,6 +2260,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C20C73FF-AAF1-4BDD-9C40-B4772DF82186}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7BCD6B0-A36C-4B0E-9370-E7046D7BE05E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
@@ -2275,14 +2281,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C20C73FF-AAF1-4BDD-9C40-B4772DF82186}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
add limits of volumetrend and currency, update percentagegoodauc
</commit_message>
<xml_diff>
--- a/python/pdstools/resources/MetricLimits.xlsx
+++ b/python/pdstools/resources/MetricLimits.xlsx
@@ -5,22 +5,35 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pegasystems-my.sharepoint.com/personal/jonas_vanelburg_pega_com/Documents/Documents/code/pega-datascientist-tools/python/pdstools/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vanej/Code/pega-datascientist-tools/python/pdstools/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="11_31FCA897298E4FCFA60F74E9B0E2CDC1BBA97614" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{063C8731-790D-7B4A-A5E6-8EF5CB479AE5}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C114789-B34C-6B4C-84FE-0896A337E85B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18740" yWindow="-23500" windowWidth="38400" windowHeight="23500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Thresholds" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="75">
   <si>
     <t>Category</t>
   </si>
@@ -233,6 +246,18 @@
   </si>
   <si>
     <t>OutboundChannelCount</t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>How many minor versions behind the most recent version of Pega?</t>
+  </si>
+  <si>
+    <t>InboundVolumeTrend</t>
+  </si>
+  <si>
+    <t>OutboundVolumeTrend</t>
   </si>
 </sst>
 </file>
@@ -242,7 +267,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0%"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -281,6 +306,13 @@
       <name val="Menlo"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -309,7 +341,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -339,6 +371,9 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -357,8 +392,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Thresholds" displayName="Thresholds" ref="A1:G43" totalsRowShown="0">
-  <autoFilter ref="A1:G43" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Thresholds" displayName="Thresholds" ref="A1:G46" totalsRowShown="0">
+  <autoFilter ref="A1:G46" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Category"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="MetricID"/>
@@ -662,8 +697,8 @@
   </sheetPr>
   <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -786,25 +821,31 @@
     </row>
     <row r="6" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="1" t="b">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" s="11">
+        <v>0.75</v>
+      </c>
+      <c r="D6" s="12">
+        <v>0.95</v>
       </c>
       <c r="H6" s="6"/>
     </row>
     <row r="7" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="1" t="b">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" s="11">
+        <v>0.75</v>
+      </c>
+      <c r="D7" s="12">
+        <v>0.95</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>22</v>
@@ -815,9 +856,9 @@
         <v>19</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="1" t="b">
+        <v>20</v>
+      </c>
+      <c r="D8" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H8" s="6" t="s">
@@ -829,7 +870,7 @@
         <v>19</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C9" s="1" t="b">
         <v>1</v>
@@ -838,22 +879,13 @@
     </row>
     <row r="10" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="3">
-        <v>2</v>
-      </c>
-      <c r="D10" s="3">
-        <v>5</v>
-      </c>
-      <c r="E10" s="3">
-        <v>100</v>
-      </c>
-      <c r="G10" t="s">
-        <v>28</v>
+        <v>19</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="H10" s="6" t="s">
         <v>29</v>
@@ -861,31 +893,31 @@
     </row>
     <row r="11" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="3">
-        <v>1</v>
-      </c>
-      <c r="D11" s="3">
-        <v>200</v>
+        <v>25</v>
+      </c>
+      <c r="C11" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="H11" s="6"/>
     </row>
     <row r="12" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="3">
-        <v>1</v>
-      </c>
-      <c r="D12" s="3">
-        <v>200</v>
+        <v>19</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" s="1">
+        <v>-4</v>
+      </c>
+      <c r="D12" s="1">
+        <v>-2</v>
+      </c>
+      <c r="G12" t="s">
+        <v>72</v>
       </c>
       <c r="H12" s="6"/>
     </row>
@@ -894,16 +926,19 @@
         <v>26</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C13" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D13" s="3">
-        <v>200</v>
+        <v>5</v>
+      </c>
+      <c r="E13" s="3">
+        <v>100</v>
       </c>
       <c r="G13" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="H13" s="6"/>
     </row>
@@ -911,8 +946,8 @@
       <c r="A14" t="s">
         <v>26</v>
       </c>
-      <c r="B14" t="s">
-        <v>34</v>
+      <c r="B14" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="C14" s="3">
         <v>1</v>
@@ -926,14 +961,14 @@
       <c r="A15" t="s">
         <v>26</v>
       </c>
-      <c r="B15" t="s">
-        <v>35</v>
+      <c r="B15" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="C15" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15" s="3">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="H15" s="6"/>
     </row>
@@ -941,34 +976,45 @@
       <c r="A16" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>36</v>
+      <c r="B16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="3">
+        <v>1</v>
+      </c>
+      <c r="D16" s="3">
+        <v>200</v>
+      </c>
+      <c r="G16" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="D17" s="7">
-        <v>0.8</v>
-      </c>
-      <c r="E17" s="7"/>
-      <c r="G17" t="s">
-        <v>38</v>
+      <c r="B17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="3">
+        <v>1</v>
+      </c>
+      <c r="D17" s="3">
+        <v>200</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>39</v>
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="3">
+        <v>0</v>
+      </c>
+      <c r="D18" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -976,19 +1022,7 @@
         <v>26</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" s="10">
-        <v>0.52</v>
-      </c>
-      <c r="D19" s="10">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="E19" s="10">
-        <v>0.8</v>
-      </c>
-      <c r="F19" s="10">
-        <v>0.9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -996,7 +1030,17 @@
         <v>26</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
+      </c>
+      <c r="C20" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="D20" s="7">
+        <v>0.75</v>
+      </c>
+      <c r="E20" s="7"/>
+      <c r="G20" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1004,50 +1048,35 @@
         <v>26</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>26</v>
       </c>
-      <c r="B22" t="s">
-        <v>43</v>
-      </c>
-      <c r="C22" s="7">
-        <v>0.01</v>
-      </c>
-      <c r="D22" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="E22" s="7">
-        <v>1</v>
-      </c>
-      <c r="G22" t="s">
-        <v>44</v>
+      <c r="B22" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" s="10">
+        <v>0.52</v>
+      </c>
+      <c r="D22" s="10">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E22" s="10">
+        <v>0.8</v>
+      </c>
+      <c r="F22" s="10">
+        <v>0.9</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>26</v>
       </c>
-      <c r="B23" t="s">
-        <v>45</v>
-      </c>
-      <c r="C23" s="3">
-        <v>50</v>
-      </c>
-      <c r="D23" s="3">
-        <v>200</v>
-      </c>
-      <c r="E23" s="3">
-        <v>700</v>
-      </c>
-      <c r="F23" s="3">
-        <v>2000</v>
-      </c>
-      <c r="G23" t="s">
-        <v>46</v>
+      <c r="B23" s="2" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1055,73 +1084,89 @@
         <v>26</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C24" s="4">
-        <v>0.95</v>
-      </c>
-      <c r="D24" s="4">
-        <v>1.05</v>
-      </c>
-      <c r="G24" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>50</v>
-      </c>
-      <c r="C25" s="3">
-        <v>1</v>
-      </c>
-      <c r="D25" s="3">
-        <v>2</v>
+        <v>43</v>
+      </c>
+      <c r="C25" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="D25" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="E25" s="7">
+        <v>1</v>
+      </c>
+      <c r="G25" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>49</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>51</v>
+        <v>26</v>
+      </c>
+      <c r="B26" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" s="3">
+        <v>50</v>
+      </c>
+      <c r="D26" s="3">
+        <v>200</v>
+      </c>
+      <c r="E26" s="3">
+        <v>700</v>
+      </c>
+      <c r="F26" s="3">
+        <v>2000</v>
+      </c>
+      <c r="G26" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>52</v>
+        <v>47</v>
+      </c>
+      <c r="C27" s="4">
+        <v>0.95</v>
+      </c>
+      <c r="D27" s="4">
+        <v>1.05</v>
+      </c>
+      <c r="G27" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>49</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C28" s="7">
-        <v>0.2</v>
-      </c>
-      <c r="D28" s="7">
-        <v>0.9</v>
-      </c>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
+      <c r="B28" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" s="3">
+        <v>1</v>
+      </c>
+      <c r="D28" s="3">
+        <v>2</v>
+      </c>
     </row>
     <row r="29" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>49</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C29" s="1" t="b">
-        <v>1</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1129,10 +1174,7 @@
         <v>49</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D30" s="1" t="b">
-        <v>1</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1140,101 +1182,79 @@
         <v>49</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C31" s="1" t="b">
-        <v>1</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="C31" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="D31" s="7">
+        <v>0.9</v>
+      </c>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
     </row>
     <row r="32" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>49</v>
       </c>
-      <c r="B32" t="s">
-        <v>57</v>
-      </c>
-      <c r="D32" s="1" t="b">
+      <c r="B32" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C32" s="1" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C33" s="3">
-        <v>50</v>
-      </c>
-      <c r="D33" s="3">
-        <v>100</v>
-      </c>
-      <c r="E33" s="3">
-        <v>2500</v>
-      </c>
-      <c r="F33" s="3">
-        <v>10000</v>
-      </c>
-      <c r="G33" t="s">
-        <v>60</v>
+        <v>55</v>
+      </c>
+      <c r="D33" s="1" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C34" s="3">
-        <v>50</v>
-      </c>
-      <c r="D34" s="3">
-        <v>100</v>
-      </c>
-      <c r="E34" s="3">
-        <v>2500</v>
-      </c>
-      <c r="F34" s="3">
-        <v>10000</v>
+        <v>56</v>
+      </c>
+      <c r="C34" s="1" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>58</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C35" s="3">
-        <v>1</v>
-      </c>
-      <c r="D35" s="3">
-        <v>5</v>
-      </c>
-      <c r="E35" s="3">
-        <v>25</v>
-      </c>
-      <c r="G35" t="s">
-        <v>60</v>
+        <v>49</v>
+      </c>
+      <c r="B35" t="s">
+        <v>57</v>
+      </c>
+      <c r="D35" s="1" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>58</v>
       </c>
-      <c r="B36" t="s">
-        <v>63</v>
+      <c r="B36" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="C36" s="3">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="D36" s="3">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="E36" s="3">
-        <v>5</v>
+        <v>2500</v>
+      </c>
+      <c r="F36" s="3">
+        <v>10000</v>
       </c>
       <c r="G36" t="s">
         <v>60</v>
@@ -1245,41 +1265,56 @@
         <v>58</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
+      </c>
+      <c r="C37" s="3">
+        <v>50</v>
+      </c>
+      <c r="D37" s="3">
+        <v>100</v>
+      </c>
+      <c r="E37" s="3">
+        <v>2500</v>
+      </c>
+      <c r="F37" s="3">
+        <v>10000</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>58</v>
       </c>
-      <c r="B38" t="s">
-        <v>65</v>
+      <c r="B38" s="2" t="s">
+        <v>62</v>
       </c>
       <c r="C38" s="3">
         <v>1</v>
       </c>
       <c r="D38" s="3">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="E38" s="3">
-        <v>250</v>
+        <v>25</v>
+      </c>
+      <c r="G38" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>58</v>
       </c>
-      <c r="B39" s="2" t="s">
-        <v>66</v>
+      <c r="B39" t="s">
+        <v>63</v>
       </c>
       <c r="C39" s="3">
         <v>1</v>
       </c>
       <c r="D39" s="3">
+        <v>1</v>
+      </c>
+      <c r="E39" s="3">
         <v>5</v>
-      </c>
-      <c r="E39" s="3">
-        <v>25</v>
       </c>
       <c r="G39" t="s">
         <v>60</v>
@@ -1289,23 +1324,8 @@
       <c r="A40" t="s">
         <v>58</v>
       </c>
-      <c r="B40" t="s">
-        <v>67</v>
-      </c>
-      <c r="C40" s="3">
-        <v>2</v>
-      </c>
-      <c r="D40" s="3">
-        <v>2500</v>
-      </c>
-      <c r="E40" s="3">
-        <v>5000</v>
-      </c>
-      <c r="F40" s="3">
-        <v>5000</v>
-      </c>
-      <c r="G40" t="s">
-        <v>60</v>
+      <c r="B40" s="2" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1313,22 +1333,16 @@
         <v>58</v>
       </c>
       <c r="B41" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C41" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D41" s="3">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="E41" s="3">
-        <v>2500</v>
-      </c>
-      <c r="F41" s="3">
-        <v>2500</v>
-      </c>
-      <c r="G41" t="s">
-        <v>60</v>
+        <v>250</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1336,43 +1350,100 @@
         <v>58</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C42" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D42" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E42" s="3">
-        <v>50</v>
+        <v>25</v>
+      </c>
+      <c r="G42" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>58</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B43" t="s">
+        <v>67</v>
+      </c>
+      <c r="C43" s="3">
+        <v>2</v>
+      </c>
+      <c r="D43" s="3">
+        <v>2500</v>
+      </c>
+      <c r="E43" s="3">
+        <v>5000</v>
+      </c>
+      <c r="F43" s="3">
+        <v>5000</v>
+      </c>
+      <c r="G43" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>58</v>
+      </c>
+      <c r="B44" t="s">
+        <v>68</v>
+      </c>
+      <c r="C44" s="3">
+        <v>2</v>
+      </c>
+      <c r="D44" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E44" s="3">
+        <v>2500</v>
+      </c>
+      <c r="F44" s="3">
+        <v>2500</v>
+      </c>
+      <c r="G44" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>58</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C45" s="3">
+        <v>0</v>
+      </c>
+      <c r="D45" s="3">
+        <v>1</v>
+      </c>
+      <c r="E45" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>58</v>
+      </c>
+      <c r="B46" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C43" s="3">
+      <c r="C46" s="3">
         <v>0</v>
       </c>
-      <c r="D43" s="3">
-        <v>1</v>
-      </c>
-      <c r="E43" s="3">
+      <c r="D46" s="3">
+        <v>1</v>
+      </c>
+      <c r="E46" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="8"/>
-    </row>
-    <row r="45" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="8"/>
-    </row>
-    <row r="46" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="8"/>
     </row>
     <row r="47" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="8"/>

</xml_diff>

<commit_message>
Add two new metrics
</commit_message>
<xml_diff>
--- a/python/pdstools/resources/MetricLimits.xlsx
+++ b/python/pdstools/resources/MetricLimits.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vanej/Code/pega-datascientist-tools/python/pdstools/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kass1/Documents/Code/pdstools_v4/pega-datascientist-tools/python/pdstools/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C114789-B34C-6B4C-84FE-0896A337E85B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9331DEA8-064C-AA41-8CE6-2E158D42827C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="34560" windowHeight="20100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Thresholds" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="77">
   <si>
     <t>Category</t>
   </si>
@@ -258,14 +258,21 @@
   </si>
   <si>
     <t>OutboundVolumeTrend</t>
+  </si>
+  <si>
+    <t>ModelsWithoutPositivesPercentage</t>
+  </si>
+  <si>
+    <t>ModelsWithGoodAUCPercentage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0%"/>
+    <numFmt numFmtId="165" formatCode="#,##0.0"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -341,7 +348,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -374,6 +381,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -392,8 +400,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Thresholds" displayName="Thresholds" ref="A1:G46" totalsRowShown="0">
-  <autoFilter ref="A1:G46" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Thresholds" displayName="Thresholds" ref="A1:G48" totalsRowShown="0">
+  <autoFilter ref="A1:G48" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Category"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="MetricID"/>
@@ -695,10 +703,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:H62"/>
+  <dimension ref="A1:H64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="157" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1076,105 +1084,121 @@
         <v>26</v>
       </c>
       <c r="B23" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C23" s="10">
+        <v>0.3</v>
+      </c>
+      <c r="D23" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+    </row>
+    <row r="24" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24" s="2" t="s">
+    <row r="25" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" t="s">
-        <v>43</v>
-      </c>
-      <c r="C25" s="7">
-        <v>0.01</v>
-      </c>
-      <c r="D25" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="E25" s="7">
-        <v>1</v>
-      </c>
-      <c r="G25" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>26</v>
       </c>
-      <c r="B26" t="s">
-        <v>45</v>
-      </c>
-      <c r="C26" s="3">
-        <v>50</v>
-      </c>
-      <c r="D26" s="3">
-        <v>200</v>
-      </c>
-      <c r="E26" s="3">
-        <v>700</v>
-      </c>
-      <c r="F26" s="3">
-        <v>2000</v>
-      </c>
-      <c r="G26" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="F26" s="14">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C27" s="4">
-        <v>0.95</v>
-      </c>
-      <c r="D27" s="4">
-        <v>1.05</v>
+      <c r="B27" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="D27" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="E27" s="7">
+        <v>1</v>
       </c>
       <c r="G27" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="B28" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28" s="3">
         <v>50</v>
       </c>
-      <c r="C28" s="3">
-        <v>1</v>
-      </c>
       <c r="D28" s="3">
-        <v>2</v>
+        <v>200</v>
+      </c>
+      <c r="E28" s="3">
+        <v>700</v>
+      </c>
+      <c r="F28" s="3">
+        <v>2000</v>
+      </c>
+      <c r="G28" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
+      </c>
+      <c r="C29" s="4">
+        <v>0.95</v>
+      </c>
+      <c r="D29" s="4">
+        <v>1.05</v>
+      </c>
+      <c r="G29" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>49</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>52</v>
+      <c r="B30" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30" s="3">
+        <v>1</v>
+      </c>
+      <c r="D30" s="3">
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1182,45 +1206,39 @@
         <v>49</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C31" s="7">
-        <v>0.2</v>
-      </c>
-      <c r="D31" s="7">
-        <v>0.9</v>
-      </c>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-    </row>
-    <row r="32" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>49</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C32" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>49</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D33" s="1" t="b">
-        <v>1</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="C33" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="D33" s="7">
+        <v>0.9</v>
+      </c>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
     </row>
     <row r="34" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>49</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C34" s="1" t="b">
         <v>1</v>
@@ -1230,8 +1248,8 @@
       <c r="A35" t="s">
         <v>49</v>
       </c>
-      <c r="B35" t="s">
-        <v>57</v>
+      <c r="B35" s="2" t="s">
+        <v>55</v>
       </c>
       <c r="D35" s="1" t="b">
         <v>1</v>
@@ -1239,45 +1257,24 @@
     </row>
     <row r="36" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C36" s="3">
-        <v>50</v>
-      </c>
-      <c r="D36" s="3">
-        <v>100</v>
-      </c>
-      <c r="E36" s="3">
-        <v>2500</v>
-      </c>
-      <c r="F36" s="3">
-        <v>10000</v>
-      </c>
-      <c r="G36" t="s">
-        <v>60</v>
+        <v>56</v>
+      </c>
+      <c r="C36" s="1" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>58</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C37" s="3">
-        <v>50</v>
-      </c>
-      <c r="D37" s="3">
-        <v>100</v>
-      </c>
-      <c r="E37" s="3">
-        <v>2500</v>
-      </c>
-      <c r="F37" s="3">
-        <v>10000</v>
+        <v>49</v>
+      </c>
+      <c r="B37" t="s">
+        <v>57</v>
+      </c>
+      <c r="D37" s="1" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1285,16 +1282,19 @@
         <v>58</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C38" s="3">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="D38" s="3">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="E38" s="3">
-        <v>25</v>
+        <v>2500</v>
+      </c>
+      <c r="F38" s="3">
+        <v>10000</v>
       </c>
       <c r="G38" t="s">
         <v>60</v>
@@ -1304,20 +1304,20 @@
       <c r="A39" t="s">
         <v>58</v>
       </c>
-      <c r="B39" t="s">
-        <v>63</v>
+      <c r="B39" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="C39" s="3">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="D39" s="3">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="E39" s="3">
-        <v>5</v>
-      </c>
-      <c r="G39" t="s">
-        <v>60</v>
+        <v>2500</v>
+      </c>
+      <c r="F39" s="3">
+        <v>10000</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1325,7 +1325,19 @@
         <v>58</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
+      </c>
+      <c r="C40" s="3">
+        <v>1</v>
+      </c>
+      <c r="D40" s="3">
+        <v>5</v>
+      </c>
+      <c r="E40" s="3">
+        <v>25</v>
+      </c>
+      <c r="G40" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1333,16 +1345,19 @@
         <v>58</v>
       </c>
       <c r="B41" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C41" s="3">
         <v>1</v>
       </c>
       <c r="D41" s="3">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="E41" s="3">
-        <v>250</v>
+        <v>5</v>
+      </c>
+      <c r="G41" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1350,19 +1365,7 @@
         <v>58</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C42" s="3">
-        <v>1</v>
-      </c>
-      <c r="D42" s="3">
-        <v>5</v>
-      </c>
-      <c r="E42" s="3">
-        <v>25</v>
-      </c>
-      <c r="G42" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1370,42 +1373,33 @@
         <v>58</v>
       </c>
       <c r="B43" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C43" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D43" s="3">
-        <v>2500</v>
+        <v>100</v>
       </c>
       <c r="E43" s="3">
-        <v>5000</v>
-      </c>
-      <c r="F43" s="3">
-        <v>5000</v>
-      </c>
-      <c r="G43" t="s">
-        <v>60</v>
+        <v>250</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>58</v>
       </c>
-      <c r="B44" t="s">
-        <v>68</v>
+      <c r="B44" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="C44" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D44" s="3">
-        <v>1000</v>
+        <v>5</v>
       </c>
       <c r="E44" s="3">
-        <v>2500</v>
-      </c>
-      <c r="F44" s="3">
-        <v>2500</v>
+        <v>25</v>
       </c>
       <c r="G44" t="s">
         <v>60</v>
@@ -1415,41 +1409,81 @@
       <c r="A45" t="s">
         <v>58</v>
       </c>
-      <c r="B45" s="2" t="s">
-        <v>69</v>
+      <c r="B45" t="s">
+        <v>67</v>
       </c>
       <c r="C45" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D45" s="3">
-        <v>1</v>
+        <v>2500</v>
       </c>
       <c r="E45" s="3">
-        <v>50</v>
+        <v>5000</v>
+      </c>
+      <c r="F45" s="3">
+        <v>5000</v>
+      </c>
+      <c r="G45" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>58</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B46" t="s">
+        <v>68</v>
+      </c>
+      <c r="C46" s="3">
+        <v>2</v>
+      </c>
+      <c r="D46" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E46" s="3">
+        <v>2500</v>
+      </c>
+      <c r="F46" s="3">
+        <v>2500</v>
+      </c>
+      <c r="G46" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>58</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C47" s="3">
+        <v>0</v>
+      </c>
+      <c r="D47" s="3">
+        <v>1</v>
+      </c>
+      <c r="E47" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>58</v>
+      </c>
+      <c r="B48" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C46" s="3">
+      <c r="C48" s="3">
         <v>0</v>
       </c>
-      <c r="D46" s="3">
-        <v>1</v>
-      </c>
-      <c r="E46" s="3">
+      <c r="D48" s="3">
+        <v>1</v>
+      </c>
+      <c r="E48" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="8"/>
-    </row>
-    <row r="48" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="8"/>
     </row>
     <row r="49" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="8"/>
@@ -1467,13 +1501,13 @@
       <c r="A53" s="8"/>
     </row>
     <row r="54" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="9"/>
+      <c r="A54" s="8"/>
     </row>
     <row r="55" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="8"/>
     </row>
     <row r="56" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="8"/>
+      <c r="A56" s="9"/>
     </row>
     <row r="57" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="8"/>
@@ -1492,6 +1526,12 @@
     </row>
     <row r="62" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="8"/>
+    </row>
+    <row r="63" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="8"/>
+    </row>
+    <row r="64" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
I shouldn't make typos.
</commit_message>
<xml_diff>
--- a/python/pdstools/resources/MetricLimits.xlsx
+++ b/python/pdstools/resources/MetricLimits.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kass1/Documents/Code/pdstools_v4/pega-datascientist-tools/python/pdstools/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9331DEA8-064C-AA41-8CE6-2E158D42827C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E55D9929-3728-CB49-A255-8CFD67AD8FEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="34560" windowHeight="20100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -260,10 +260,10 @@
     <t>OutboundVolumeTrend</t>
   </si>
   <si>
-    <t>ModelsWithoutPositivesPercentage</t>
-  </si>
-  <si>
     <t>ModelsWithGoodAUCPercentage</t>
+  </si>
+  <si>
+    <t>ModelsWithoutResponsesPercentage</t>
   </si>
 </sst>
 </file>
@@ -705,8 +705,8 @@
   </sheetPr>
   <dimension ref="A1:H64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="157" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="157" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1084,7 +1084,7 @@
         <v>26</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C23" s="10">
         <v>0.3</v>
@@ -1116,7 +1116,7 @@
         <v>26</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C26" s="14"/>
       <c r="D26" s="14"/>

</xml_diff>

<commit_message>
Add two new metrics to the limits file (#518)
* Add two new metrics

* Auto-export CSV from Excel table

* I shouldn't make typos.

* Auto-export CSV from Excel table

---------

Co-authored-by: github-actions[bot] <github-actions[bot]@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/python/pdstools/resources/MetricLimits.xlsx
+++ b/python/pdstools/resources/MetricLimits.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vanej/Code/pega-datascientist-tools/python/pdstools/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kass1/Documents/Code/pdstools_v4/pega-datascientist-tools/python/pdstools/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C114789-B34C-6B4C-84FE-0896A337E85B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E55D9929-3728-CB49-A255-8CFD67AD8FEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="34560" windowHeight="20100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Thresholds" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="77">
   <si>
     <t>Category</t>
   </si>
@@ -258,14 +258,21 @@
   </si>
   <si>
     <t>OutboundVolumeTrend</t>
+  </si>
+  <si>
+    <t>ModelsWithGoodAUCPercentage</t>
+  </si>
+  <si>
+    <t>ModelsWithoutResponsesPercentage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0%"/>
+    <numFmt numFmtId="165" formatCode="#,##0.0"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -341,7 +348,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -374,6 +381,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -392,8 +400,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Thresholds" displayName="Thresholds" ref="A1:G46" totalsRowShown="0">
-  <autoFilter ref="A1:G46" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Thresholds" displayName="Thresholds" ref="A1:G48" totalsRowShown="0">
+  <autoFilter ref="A1:G48" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Category"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="MetricID"/>
@@ -695,10 +703,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:H62"/>
+  <dimension ref="A1:H64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="157" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1076,105 +1084,121 @@
         <v>26</v>
       </c>
       <c r="B23" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C23" s="10">
+        <v>0.3</v>
+      </c>
+      <c r="D23" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+    </row>
+    <row r="24" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24" s="2" t="s">
+    <row r="25" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" t="s">
-        <v>43</v>
-      </c>
-      <c r="C25" s="7">
-        <v>0.01</v>
-      </c>
-      <c r="D25" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="E25" s="7">
-        <v>1</v>
-      </c>
-      <c r="G25" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>26</v>
       </c>
-      <c r="B26" t="s">
-        <v>45</v>
-      </c>
-      <c r="C26" s="3">
-        <v>50</v>
-      </c>
-      <c r="D26" s="3">
-        <v>200</v>
-      </c>
-      <c r="E26" s="3">
-        <v>700</v>
-      </c>
-      <c r="F26" s="3">
-        <v>2000</v>
-      </c>
-      <c r="G26" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="F26" s="14">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C27" s="4">
-        <v>0.95</v>
-      </c>
-      <c r="D27" s="4">
-        <v>1.05</v>
+      <c r="B27" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="D27" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="E27" s="7">
+        <v>1</v>
       </c>
       <c r="G27" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="B28" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28" s="3">
         <v>50</v>
       </c>
-      <c r="C28" s="3">
-        <v>1</v>
-      </c>
       <c r="D28" s="3">
-        <v>2</v>
+        <v>200</v>
+      </c>
+      <c r="E28" s="3">
+        <v>700</v>
+      </c>
+      <c r="F28" s="3">
+        <v>2000</v>
+      </c>
+      <c r="G28" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
+      </c>
+      <c r="C29" s="4">
+        <v>0.95</v>
+      </c>
+      <c r="D29" s="4">
+        <v>1.05</v>
+      </c>
+      <c r="G29" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>49</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>52</v>
+      <c r="B30" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30" s="3">
+        <v>1</v>
+      </c>
+      <c r="D30" s="3">
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1182,45 +1206,39 @@
         <v>49</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C31" s="7">
-        <v>0.2</v>
-      </c>
-      <c r="D31" s="7">
-        <v>0.9</v>
-      </c>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-    </row>
-    <row r="32" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>49</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C32" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>49</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D33" s="1" t="b">
-        <v>1</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="C33" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="D33" s="7">
+        <v>0.9</v>
+      </c>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
     </row>
     <row r="34" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>49</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C34" s="1" t="b">
         <v>1</v>
@@ -1230,8 +1248,8 @@
       <c r="A35" t="s">
         <v>49</v>
       </c>
-      <c r="B35" t="s">
-        <v>57</v>
+      <c r="B35" s="2" t="s">
+        <v>55</v>
       </c>
       <c r="D35" s="1" t="b">
         <v>1</v>
@@ -1239,45 +1257,24 @@
     </row>
     <row r="36" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C36" s="3">
-        <v>50</v>
-      </c>
-      <c r="D36" s="3">
-        <v>100</v>
-      </c>
-      <c r="E36" s="3">
-        <v>2500</v>
-      </c>
-      <c r="F36" s="3">
-        <v>10000</v>
-      </c>
-      <c r="G36" t="s">
-        <v>60</v>
+        <v>56</v>
+      </c>
+      <c r="C36" s="1" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>58</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C37" s="3">
-        <v>50</v>
-      </c>
-      <c r="D37" s="3">
-        <v>100</v>
-      </c>
-      <c r="E37" s="3">
-        <v>2500</v>
-      </c>
-      <c r="F37" s="3">
-        <v>10000</v>
+        <v>49</v>
+      </c>
+      <c r="B37" t="s">
+        <v>57</v>
+      </c>
+      <c r="D37" s="1" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1285,16 +1282,19 @@
         <v>58</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C38" s="3">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="D38" s="3">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="E38" s="3">
-        <v>25</v>
+        <v>2500</v>
+      </c>
+      <c r="F38" s="3">
+        <v>10000</v>
       </c>
       <c r="G38" t="s">
         <v>60</v>
@@ -1304,20 +1304,20 @@
       <c r="A39" t="s">
         <v>58</v>
       </c>
-      <c r="B39" t="s">
-        <v>63</v>
+      <c r="B39" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="C39" s="3">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="D39" s="3">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="E39" s="3">
-        <v>5</v>
-      </c>
-      <c r="G39" t="s">
-        <v>60</v>
+        <v>2500</v>
+      </c>
+      <c r="F39" s="3">
+        <v>10000</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1325,7 +1325,19 @@
         <v>58</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
+      </c>
+      <c r="C40" s="3">
+        <v>1</v>
+      </c>
+      <c r="D40" s="3">
+        <v>5</v>
+      </c>
+      <c r="E40" s="3">
+        <v>25</v>
+      </c>
+      <c r="G40" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1333,16 +1345,19 @@
         <v>58</v>
       </c>
       <c r="B41" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C41" s="3">
         <v>1</v>
       </c>
       <c r="D41" s="3">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="E41" s="3">
-        <v>250</v>
+        <v>5</v>
+      </c>
+      <c r="G41" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1350,19 +1365,7 @@
         <v>58</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C42" s="3">
-        <v>1</v>
-      </c>
-      <c r="D42" s="3">
-        <v>5</v>
-      </c>
-      <c r="E42" s="3">
-        <v>25</v>
-      </c>
-      <c r="G42" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1370,42 +1373,33 @@
         <v>58</v>
       </c>
       <c r="B43" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C43" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D43" s="3">
-        <v>2500</v>
+        <v>100</v>
       </c>
       <c r="E43" s="3">
-        <v>5000</v>
-      </c>
-      <c r="F43" s="3">
-        <v>5000</v>
-      </c>
-      <c r="G43" t="s">
-        <v>60</v>
+        <v>250</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>58</v>
       </c>
-      <c r="B44" t="s">
-        <v>68</v>
+      <c r="B44" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="C44" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D44" s="3">
-        <v>1000</v>
+        <v>5</v>
       </c>
       <c r="E44" s="3">
-        <v>2500</v>
-      </c>
-      <c r="F44" s="3">
-        <v>2500</v>
+        <v>25</v>
       </c>
       <c r="G44" t="s">
         <v>60</v>
@@ -1415,41 +1409,81 @@
       <c r="A45" t="s">
         <v>58</v>
       </c>
-      <c r="B45" s="2" t="s">
-        <v>69</v>
+      <c r="B45" t="s">
+        <v>67</v>
       </c>
       <c r="C45" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D45" s="3">
-        <v>1</v>
+        <v>2500</v>
       </c>
       <c r="E45" s="3">
-        <v>50</v>
+        <v>5000</v>
+      </c>
+      <c r="F45" s="3">
+        <v>5000</v>
+      </c>
+      <c r="G45" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>58</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B46" t="s">
+        <v>68</v>
+      </c>
+      <c r="C46" s="3">
+        <v>2</v>
+      </c>
+      <c r="D46" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E46" s="3">
+        <v>2500</v>
+      </c>
+      <c r="F46" s="3">
+        <v>2500</v>
+      </c>
+      <c r="G46" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>58</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C47" s="3">
+        <v>0</v>
+      </c>
+      <c r="D47" s="3">
+        <v>1</v>
+      </c>
+      <c r="E47" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>58</v>
+      </c>
+      <c r="B48" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C46" s="3">
+      <c r="C48" s="3">
         <v>0</v>
       </c>
-      <c r="D46" s="3">
-        <v>1</v>
-      </c>
-      <c r="E46" s="3">
+      <c r="D48" s="3">
+        <v>1</v>
+      </c>
+      <c r="E48" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="8"/>
-    </row>
-    <row r="48" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="8"/>
     </row>
     <row r="49" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="8"/>
@@ -1467,13 +1501,13 @@
       <c r="A53" s="8"/>
     </row>
     <row r="54" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="9"/>
+      <c r="A54" s="8"/>
     </row>
     <row r="55" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="8"/>
     </row>
     <row r="56" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="8"/>
+      <c r="A56" s="9"/>
     </row>
     <row r="57" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="8"/>
@@ -1492,6 +1526,12 @@
     </row>
     <row r="62" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="8"/>
+    </row>
+    <row r="63" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="8"/>
+    </row>
+    <row r="64" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Increase the minimum models with good AUC percentage threshold
</commit_message>
<xml_diff>
--- a/python/pdstools/resources/MetricLimits.xlsx
+++ b/python/pdstools/resources/MetricLimits.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kass1/Documents/Code/pdstools_v4/pega-datascientist-tools/python/pdstools/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E55D9929-3728-CB49-A255-8CFD67AD8FEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B7D033C-1DA4-8543-B0E1-A332D4DD7A44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="34560" windowHeight="20100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -705,8 +705,8 @@
   </sheetPr>
   <dimension ref="A1:H64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="157" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="157" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1087,10 +1087,10 @@
         <v>75</v>
       </c>
       <c r="C23" s="10">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="D23" s="10">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="E23" s="10"/>
       <c r="F23" s="10"/>

</xml_diff>

<commit_message>
Increase percentage of models with good AUC in limits file (#519)
* Increase the minimum models with good AUC percentage threshold

* Auto-export CSV from Excel table

---------

Co-authored-by: github-actions[bot] <github-actions[bot]@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/python/pdstools/resources/MetricLimits.xlsx
+++ b/python/pdstools/resources/MetricLimits.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kass1/Documents/Code/pdstools_v4/pega-datascientist-tools/python/pdstools/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E55D9929-3728-CB49-A255-8CFD67AD8FEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B7D033C-1DA4-8543-B0E1-A332D4DD7A44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="34560" windowHeight="20100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -705,8 +705,8 @@
   </sheetPr>
   <dimension ref="A1:H64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="157" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="157" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1087,10 +1087,10 @@
         <v>75</v>
       </c>
       <c r="C23" s="10">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="D23" s="10">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="E23" s="10"/>
       <c r="F23" s="10"/>

</xml_diff>